<commit_message>
Laporan 2023.08.24 / Rename Folder dan File
</commit_message>
<xml_diff>
--- a/LAPORAN PENGAMBILAN MATERIAL DEPT KABEL/LAPORAN PENGAMBILAN MATERIAL DEPT KABEL.xlsx
+++ b/LAPORAN PENGAMBILAN MATERIAL DEPT KABEL/LAPORAN PENGAMBILAN MATERIAL DEPT KABEL.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="48">
   <si>
     <t>TANGGAL</t>
   </si>
@@ -372,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -462,7 +462,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,91 +516,74 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -889,66 +913,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="49" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="36"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="49"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1013,11 +1037,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
+      <pane ySplit="5" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,87 +1058,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="49" t="s">
         <v>4</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="36"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="49"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
@@ -1146,10 +1170,10 @@
       <c r="A7" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="50">
+      <c r="B7" s="55">
         <v>45145</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="60">
         <v>20230805001</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1179,8 +1203,8 @@
       <c r="A8" s="3">
         <v>2</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1205,8 +1229,8 @@
       <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1220,7 +1244,7 @@
       <c r="H9" s="3">
         <v>25</v>
       </c>
-      <c r="I9" s="66">
+      <c r="I9" s="41">
         <f t="shared" ref="I9:I16" si="0">SUM(H9-G9)</f>
         <v>9.5</v>
       </c>
@@ -1232,8 +1256,8 @@
       <c r="A10" s="3">
         <v>4</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1247,7 +1271,7 @@
       <c r="H10" s="7">
         <v>25</v>
       </c>
-      <c r="I10" s="66">
+      <c r="I10" s="41">
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
@@ -1259,8 +1283,8 @@
       <c r="A11" s="3">
         <v>5</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1298,7 @@
       <c r="H11" s="7">
         <v>25</v>
       </c>
-      <c r="I11" s="66">
+      <c r="I11" s="41">
         <f t="shared" si="0"/>
         <v>4.4699999999999989</v>
       </c>
@@ -1286,8 +1310,8 @@
       <c r="A12" s="3">
         <v>6</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="7" t="s">
         <v>22</v>
       </c>
@@ -1311,8 +1335,8 @@
       <c r="A13" s="3">
         <v>7</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="7" t="s">
         <v>23</v>
       </c>
@@ -1336,8 +1360,8 @@
       <c r="A14" s="3">
         <v>8</v>
       </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="55"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="61"/>
       <c r="D14" s="7" t="s">
         <v>29</v>
       </c>
@@ -1363,8 +1387,8 @@
       <c r="A15" s="3">
         <v>9</v>
       </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="7" t="s">
         <v>32</v>
       </c>
@@ -1390,8 +1414,8 @@
       <c r="A16" s="6">
         <v>10</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="56"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="9" t="s">
         <v>6</v>
       </c>
@@ -1439,7 +1463,7 @@
       <c r="A18" s="10">
         <v>1</v>
       </c>
-      <c r="B18" s="50">
+      <c r="B18" s="55">
         <v>45147</v>
       </c>
       <c r="C18" s="18">
@@ -1465,8 +1489,8 @@
       <c r="A19" s="7">
         <v>2</v>
       </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="41">
+      <c r="B19" s="56"/>
+      <c r="C19" s="53">
         <v>20230809003</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -1496,8 +1520,8 @@
       <c r="A20" s="7">
         <v>3</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="39"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="63"/>
       <c r="D20" s="7" t="s">
         <v>38</v>
       </c>
@@ -1525,8 +1549,8 @@
       <c r="A21" s="7">
         <v>4</v>
       </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="54"/>
       <c r="D21" s="7" t="s">
         <v>16</v>
       </c>
@@ -1554,8 +1578,8 @@
       <c r="A22" s="7">
         <v>5</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="41">
+      <c r="B22" s="56"/>
+      <c r="C22" s="53">
         <v>20230809002</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -1585,8 +1609,8 @@
       <c r="A23" s="7">
         <v>6</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="39"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="63"/>
       <c r="D23" s="7" t="s">
         <v>38</v>
       </c>
@@ -1602,7 +1626,7 @@
       <c r="H23" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I23" s="57">
+      <c r="I23" s="33">
         <f>I20-G23</f>
         <v>0.51000000000000068</v>
       </c>
@@ -1612,8 +1636,8 @@
       <c r="A24" s="7">
         <v>7</v>
       </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="40"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="54"/>
       <c r="D24" s="7" t="s">
         <v>16</v>
       </c>
@@ -1641,8 +1665,8 @@
       <c r="A25" s="7">
         <v>8</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="41">
+      <c r="B25" s="56"/>
+      <c r="C25" s="53">
         <v>20230809004</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -1672,8 +1696,8 @@
       <c r="A26" s="7">
         <v>9</v>
       </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="40"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="54"/>
       <c r="D26" s="7" t="s">
         <v>43</v>
       </c>
@@ -1701,8 +1725,8 @@
       <c r="A27" s="7">
         <v>10</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="41">
+      <c r="B27" s="56"/>
+      <c r="C27" s="53">
         <v>20230809005</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -1732,8 +1756,8 @@
       <c r="A28" s="7">
         <v>11</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="40"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="54"/>
       <c r="D28" s="7" t="s">
         <v>43</v>
       </c>
@@ -1749,7 +1773,7 @@
       <c r="H28" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I28" s="57">
+      <c r="I28" s="33">
         <f>I26-G28</f>
         <v>0.8300000000000054</v>
       </c>
@@ -1759,8 +1783,8 @@
       <c r="A29" s="7">
         <v>12</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="41">
+      <c r="B29" s="56"/>
+      <c r="C29" s="53">
         <v>20230809006</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -1778,18 +1802,20 @@
       <c r="H29" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I29" s="57">
+      <c r="I29" s="26">
         <f>I24-G29</f>
         <v>2.6899999999999995</v>
       </c>
-      <c r="J29" s="3"/>
+      <c r="J29" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>13</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="53"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="68"/>
       <c r="D30" s="9" t="s">
         <v>15</v>
       </c>
@@ -1805,11 +1831,12 @@
       <c r="H30" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="I30" s="60">
-        <f>I27-G30</f>
-        <v>-11.559999999999999</v>
-      </c>
-      <c r="J30" s="6"/>
+      <c r="I30" s="19">
+        <v>0</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
@@ -1841,7 +1868,7 @@
       <c r="A32" s="29">
         <v>1</v>
       </c>
-      <c r="B32" s="50">
+      <c r="B32" s="55">
         <v>45154</v>
       </c>
       <c r="C32" s="30"/>
@@ -1867,8 +1894,8 @@
       <c r="A33" s="7">
         <v>2</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="41">
+      <c r="B33" s="56"/>
+      <c r="C33" s="53">
         <v>20230809003</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -1896,8 +1923,8 @@
       <c r="A34" s="7">
         <v>3</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="39"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="63"/>
       <c r="D34" s="3" t="s">
         <v>20</v>
       </c>
@@ -1923,8 +1950,8 @@
       <c r="A35" s="7">
         <v>4</v>
       </c>
-      <c r="B35" s="51"/>
-      <c r="C35" s="39"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="63"/>
       <c r="D35" s="7" t="s">
         <v>21</v>
       </c>
@@ -1950,8 +1977,8 @@
       <c r="A36" s="7">
         <v>5</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="39"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="63"/>
       <c r="D36" s="7" t="s">
         <v>22</v>
       </c>
@@ -1975,8 +2002,8 @@
       <c r="A37" s="7">
         <v>6</v>
       </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="39"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="63"/>
       <c r="D37" s="7" t="s">
         <v>23</v>
       </c>
@@ -2000,8 +2027,8 @@
       <c r="A38" s="7">
         <v>7</v>
       </c>
-      <c r="B38" s="51"/>
-      <c r="C38" s="40"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="54"/>
       <c r="D38" s="7" t="s">
         <v>29</v>
       </c>
@@ -2027,8 +2054,8 @@
       <c r="A39" s="7">
         <v>8</v>
       </c>
-      <c r="B39" s="51"/>
-      <c r="C39" s="46">
+      <c r="B39" s="56"/>
+      <c r="C39" s="64">
         <v>20230809002</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2045,7 +2072,7 @@
         <v>41</v>
       </c>
       <c r="I39" s="19">
-        <f>I33-G39</f>
+        <f t="shared" ref="I39:I50" si="1">I33-G39</f>
         <v>24.04</v>
       </c>
       <c r="J39" s="19" t="s">
@@ -2056,8 +2083,8 @@
       <c r="A40" s="7">
         <v>9</v>
       </c>
-      <c r="B40" s="51"/>
-      <c r="C40" s="47"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="3" t="s">
         <v>20</v>
       </c>
@@ -2072,7 +2099,7 @@
         <v>41</v>
       </c>
       <c r="I40" s="19">
-        <f>I34-G40</f>
+        <f t="shared" si="1"/>
         <v>24.04</v>
       </c>
       <c r="J40" s="19" t="s">
@@ -2083,8 +2110,8 @@
       <c r="A41" s="7">
         <v>10</v>
       </c>
-      <c r="B41" s="51"/>
-      <c r="C41" s="47"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="65"/>
       <c r="D41" s="7" t="s">
         <v>21</v>
       </c>
@@ -2099,7 +2126,7 @@
         <v>41</v>
       </c>
       <c r="I41" s="19">
-        <f>I35-G41</f>
+        <f t="shared" si="1"/>
         <v>20.060000000000002</v>
       </c>
       <c r="J41" s="19" t="s">
@@ -2110,8 +2137,8 @@
       <c r="A42" s="7">
         <v>11</v>
       </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="47"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="65"/>
       <c r="D42" s="7" t="s">
         <v>22</v>
       </c>
@@ -2124,7 +2151,7 @@
         <v>41</v>
       </c>
       <c r="I42" s="19">
-        <f>I36-G42</f>
+        <f t="shared" si="1"/>
         <v>24.599999999999998</v>
       </c>
       <c r="J42" s="19" t="s">
@@ -2135,8 +2162,8 @@
       <c r="A43" s="7">
         <v>12</v>
       </c>
-      <c r="B43" s="51"/>
-      <c r="C43" s="47"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="65"/>
       <c r="D43" s="7" t="s">
         <v>23</v>
       </c>
@@ -2149,7 +2176,7 @@
         <v>41</v>
       </c>
       <c r="I43" s="19">
-        <f>I37-G43</f>
+        <f t="shared" si="1"/>
         <v>24.599999999999998</v>
       </c>
       <c r="J43" s="19" t="s">
@@ -2160,8 +2187,8 @@
       <c r="A44" s="7">
         <v>13</v>
       </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="48"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="66"/>
       <c r="D44" s="7" t="s">
         <v>29</v>
       </c>
@@ -2176,7 +2203,7 @@
         <v>41</v>
       </c>
       <c r="I44" s="19">
-        <f>I38-G44</f>
+        <f t="shared" si="1"/>
         <v>48.76</v>
       </c>
       <c r="J44" s="19" t="s">
@@ -2187,8 +2214,8 @@
       <c r="A45" s="7">
         <v>14</v>
       </c>
-      <c r="B45" s="51"/>
-      <c r="C45" s="46">
+      <c r="B45" s="56"/>
+      <c r="C45" s="64">
         <v>20230809006</v>
       </c>
       <c r="D45" s="3" t="s">
@@ -2204,18 +2231,20 @@
       <c r="H45" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I45" s="58">
-        <f>I39-G45</f>
+      <c r="I45" s="42">
+        <f t="shared" si="1"/>
         <v>20.96</v>
       </c>
-      <c r="J45" s="8"/>
+      <c r="J45" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>15</v>
       </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="47"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="3" t="s">
         <v>20</v>
       </c>
@@ -2229,18 +2258,20 @@
       <c r="H46" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I46" s="58">
-        <f>I40-G46</f>
+      <c r="I46" s="42">
+        <f t="shared" si="1"/>
         <v>20.96</v>
       </c>
-      <c r="J46" s="8"/>
+      <c r="J46" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>16</v>
       </c>
-      <c r="B47" s="51"/>
-      <c r="C47" s="47"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="65"/>
       <c r="D47" s="7" t="s">
         <v>21</v>
       </c>
@@ -2254,18 +2285,20 @@
       <c r="H47" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I47" s="58">
-        <f>I41-G47</f>
+      <c r="I47" s="42">
+        <f t="shared" si="1"/>
         <v>15.970000000000002</v>
       </c>
-      <c r="J47" s="8"/>
+      <c r="J47" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>17</v>
       </c>
-      <c r="B48" s="51"/>
-      <c r="C48" s="47"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="65"/>
       <c r="D48" s="7" t="s">
         <v>22</v>
       </c>
@@ -2277,8 +2310,8 @@
       <c r="H48" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I48" s="58">
-        <f>I42-G48</f>
+      <c r="I48" s="34">
+        <f t="shared" si="1"/>
         <v>24.549999999999997</v>
       </c>
       <c r="J48" s="8"/>
@@ -2287,8 +2320,8 @@
       <c r="A49" s="7">
         <v>18</v>
       </c>
-      <c r="B49" s="51"/>
-      <c r="C49" s="47"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="65"/>
       <c r="D49" s="7" t="s">
         <v>23</v>
       </c>
@@ -2300,8 +2333,8 @@
       <c r="H49" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I49" s="58">
-        <f>I43-G49</f>
+      <c r="I49" s="34">
+        <f t="shared" si="1"/>
         <v>24.549999999999997</v>
       </c>
       <c r="J49" s="8"/>
@@ -2310,8 +2343,8 @@
       <c r="A50" s="9">
         <v>19</v>
       </c>
-      <c r="B50" s="52"/>
-      <c r="C50" s="49"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="67"/>
       <c r="D50" s="9" t="s">
         <v>29</v>
       </c>
@@ -2325,20 +2358,22 @@
       <c r="H50" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="I50" s="59">
-        <f>I44-G50</f>
+      <c r="I50" s="35">
+        <f t="shared" si="1"/>
         <v>0.62999999999999545</v>
       </c>
-      <c r="J50" s="32"/>
+      <c r="J50" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>1</v>
       </c>
-      <c r="B51" s="50">
+      <c r="B51" s="55">
         <v>45157</v>
       </c>
-      <c r="C51" s="38">
+      <c r="C51" s="69">
         <v>20230816001</v>
       </c>
       <c r="D51" s="30" t="s">
@@ -2356,11 +2391,11 @@
       <c r="H51" s="30">
         <v>154.02000000000001</v>
       </c>
-      <c r="I51" s="63">
+      <c r="I51" s="38">
         <f>H51-G51</f>
         <v>78.580000000000013</v>
       </c>
-      <c r="J51" s="64" t="s">
+      <c r="J51" s="39" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2368,8 +2403,8 @@
       <c r="A52" s="4">
         <v>2</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="39"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="63"/>
       <c r="D52" s="3" t="s">
         <v>32</v>
       </c>
@@ -2395,8 +2430,8 @@
       <c r="A53" s="4">
         <v>3</v>
       </c>
-      <c r="B53" s="51"/>
-      <c r="C53" s="40"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="54"/>
       <c r="D53" s="3" t="s">
         <v>6</v>
       </c>
@@ -2424,8 +2459,8 @@
       <c r="A54" s="4">
         <v>4</v>
       </c>
-      <c r="B54" s="51"/>
-      <c r="C54" s="41">
+      <c r="B54" s="56"/>
+      <c r="C54" s="53">
         <v>20230816002</v>
       </c>
       <c r="D54" s="4" t="s">
@@ -2444,7 +2479,7 @@
         <v>41</v>
       </c>
       <c r="I54" s="27">
-        <f>I51-G54</f>
+        <f t="shared" ref="I54:I59" si="2">I51-G54</f>
         <v>59.860000000000014</v>
       </c>
       <c r="J54" s="19" t="s">
@@ -2455,8 +2490,8 @@
       <c r="A55" s="4">
         <v>5</v>
       </c>
-      <c r="B55" s="51"/>
-      <c r="C55" s="39"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="63"/>
       <c r="D55" s="3" t="s">
         <v>32</v>
       </c>
@@ -2471,7 +2506,7 @@
         <v>41</v>
       </c>
       <c r="I55" s="27">
-        <f>I52-G55</f>
+        <f t="shared" si="2"/>
         <v>10.910000000000004</v>
       </c>
       <c r="J55" s="19" t="s">
@@ -2482,8 +2517,8 @@
       <c r="A56" s="4">
         <v>6</v>
       </c>
-      <c r="B56" s="51"/>
-      <c r="C56" s="40"/>
+      <c r="B56" s="56"/>
+      <c r="C56" s="54"/>
       <c r="D56" s="3" t="s">
         <v>6</v>
       </c>
@@ -2500,7 +2535,7 @@
         <v>41</v>
       </c>
       <c r="I56" s="27">
-        <f>I53-G56</f>
+        <f t="shared" si="2"/>
         <v>58.699999999999996</v>
       </c>
       <c r="J56" s="19" t="s">
@@ -2511,8 +2546,8 @@
       <c r="A57" s="4">
         <v>7</v>
       </c>
-      <c r="B57" s="51"/>
-      <c r="C57" s="41">
+      <c r="B57" s="56"/>
+      <c r="C57" s="53">
         <v>20230816003</v>
       </c>
       <c r="D57" s="4" t="s">
@@ -2530,8 +2565,8 @@
       <c r="H57" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I57" s="57">
-        <f>I54-G57</f>
+      <c r="I57" s="33">
+        <f t="shared" si="2"/>
         <v>3.2500000000000142</v>
       </c>
       <c r="J57" s="3"/>
@@ -2540,8 +2575,8 @@
       <c r="A58" s="4">
         <v>8</v>
       </c>
-      <c r="B58" s="51"/>
-      <c r="C58" s="39"/>
+      <c r="B58" s="56"/>
+      <c r="C58" s="63"/>
       <c r="D58" s="3" t="s">
         <v>32</v>
       </c>
@@ -2556,7 +2591,7 @@
         <v>41</v>
       </c>
       <c r="I58" s="27">
-        <f>I55-G58</f>
+        <f t="shared" si="2"/>
         <v>5.7900000000000036</v>
       </c>
       <c r="J58" s="19" t="s">
@@ -2567,8 +2602,8 @@
       <c r="A59" s="4">
         <v>9</v>
       </c>
-      <c r="B59" s="51"/>
-      <c r="C59" s="40"/>
+      <c r="B59" s="56"/>
+      <c r="C59" s="54"/>
       <c r="D59" s="3" t="s">
         <v>6</v>
       </c>
@@ -2585,7 +2620,7 @@
         <v>41</v>
       </c>
       <c r="I59" s="27">
-        <f>I56-G59</f>
+        <f t="shared" si="2"/>
         <v>28.929999999999996</v>
       </c>
       <c r="J59" s="19" t="s">
@@ -2596,8 +2631,8 @@
       <c r="A60" s="4">
         <v>10</v>
       </c>
-      <c r="B60" s="51"/>
-      <c r="C60" s="42">
+      <c r="B60" s="56"/>
+      <c r="C60" s="51">
         <v>20230809002</v>
       </c>
       <c r="D60" s="7" t="s">
@@ -2614,7 +2649,7 @@
         <v>41</v>
       </c>
       <c r="I60" s="27">
-        <f>I58-G60</f>
+        <f t="shared" ref="I60:I65" si="3">I58-G60</f>
         <v>5.2500000000000036</v>
       </c>
       <c r="J60" s="19" t="s">
@@ -2625,8 +2660,8 @@
       <c r="A61" s="4">
         <v>11</v>
       </c>
-      <c r="B61" s="51"/>
-      <c r="C61" s="43"/>
+      <c r="B61" s="56"/>
+      <c r="C61" s="52"/>
       <c r="D61" s="7" t="s">
         <v>6</v>
       </c>
@@ -2643,7 +2678,7 @@
         <v>41</v>
       </c>
       <c r="I61" s="27">
-        <f>I59-G61</f>
+        <f t="shared" si="3"/>
         <v>25.809999999999995</v>
       </c>
       <c r="J61" s="19" t="s">
@@ -2654,8 +2689,8 @@
       <c r="A62" s="4">
         <v>12</v>
       </c>
-      <c r="B62" s="51"/>
-      <c r="C62" s="41">
+      <c r="B62" s="56"/>
+      <c r="C62" s="53">
         <v>20230809003</v>
       </c>
       <c r="D62" s="7" t="s">
@@ -2672,7 +2707,7 @@
         <v>41</v>
       </c>
       <c r="I62" s="27">
-        <f>I60-G62</f>
+        <f t="shared" si="3"/>
         <v>1.8400000000000034</v>
       </c>
       <c r="J62" s="19" t="s">
@@ -2683,8 +2718,8 @@
       <c r="A63" s="4">
         <v>13</v>
       </c>
-      <c r="B63" s="51"/>
-      <c r="C63" s="40"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="54"/>
       <c r="D63" s="7" t="s">
         <v>6</v>
       </c>
@@ -2701,7 +2736,7 @@
         <v>41</v>
       </c>
       <c r="I63" s="27">
-        <f>I61-G63</f>
+        <f t="shared" si="3"/>
         <v>5.9699999999999953</v>
       </c>
       <c r="J63" s="19" t="s">
@@ -2712,8 +2747,8 @@
       <c r="A64" s="4">
         <v>14</v>
       </c>
-      <c r="B64" s="51"/>
-      <c r="C64" s="41">
+      <c r="B64" s="56"/>
+      <c r="C64" s="53">
         <v>20230809006</v>
       </c>
       <c r="D64" s="7" t="s">
@@ -2729,8 +2764,8 @@
       <c r="H64" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I64" s="57">
-        <f>I62-G64</f>
+      <c r="I64" s="33">
+        <f t="shared" si="3"/>
         <v>0.17000000000000348</v>
       </c>
       <c r="J64" s="3"/>
@@ -2739,8 +2774,8 @@
       <c r="A65" s="4">
         <v>15</v>
       </c>
-      <c r="B65" s="51"/>
-      <c r="C65" s="40"/>
+      <c r="B65" s="56"/>
+      <c r="C65" s="54"/>
       <c r="D65" s="7" t="s">
         <v>6</v>
       </c>
@@ -2756,8 +2791,8 @@
       <c r="H65" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I65" s="57">
-        <f>I63-G65</f>
+      <c r="I65" s="33">
+        <f t="shared" si="3"/>
         <v>0.86999999999999567</v>
       </c>
       <c r="J65" s="3"/>
@@ -2766,7 +2801,7 @@
       <c r="A66" s="4">
         <v>16</v>
       </c>
-      <c r="B66" s="51"/>
+      <c r="B66" s="56"/>
       <c r="C66" s="3">
         <v>20230809004</v>
       </c>
@@ -2795,7 +2830,7 @@
       <c r="A67" s="4">
         <v>17</v>
       </c>
-      <c r="B67" s="51"/>
+      <c r="B67" s="56"/>
       <c r="C67" s="3">
         <v>20230809005</v>
       </c>
@@ -2812,7 +2847,7 @@
       <c r="H67" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I67" s="62">
+      <c r="I67" s="37">
         <f>I66-G67</f>
         <v>60.100000000000009</v>
       </c>
@@ -2822,7 +2857,7 @@
       <c r="A68" s="4">
         <v>18</v>
       </c>
-      <c r="B68" s="51"/>
+      <c r="B68" s="56"/>
       <c r="C68" s="3">
         <v>20230814001</v>
       </c>
@@ -2839,7 +2874,7 @@
       <c r="H68" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I68" s="61">
+      <c r="I68" s="36">
         <f>I67-G68</f>
         <v>-3.8599999999999923</v>
       </c>
@@ -2849,7 +2884,7 @@
       <c r="A69" s="17">
         <v>19</v>
       </c>
-      <c r="B69" s="52"/>
+      <c r="B69" s="57"/>
       <c r="C69" s="6">
         <v>20230814001</v>
       </c>
@@ -2868,30 +2903,427 @@
       <c r="H69" s="6">
         <v>77.44</v>
       </c>
-      <c r="I69" s="65">
+      <c r="I69" s="40">
         <f>H69-G69</f>
         <v>-4.2000000000000028</v>
       </c>
       <c r="J69" s="32"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C70" s="33"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="33"/>
+      <c r="A70" s="30">
+        <v>1</v>
+      </c>
+      <c r="B70" s="55">
+        <v>45160</v>
+      </c>
+      <c r="C70" s="29">
+        <v>20230814001</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G70" s="29">
+        <v>94.9</v>
+      </c>
+      <c r="H70" s="30">
+        <v>95.77</v>
+      </c>
+      <c r="I70" s="43">
+        <f>H70-G70</f>
+        <v>0.86999999999999034</v>
+      </c>
+      <c r="J70" s="30"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
-      <c r="E71" s="33"/>
-      <c r="F71" s="33"/>
-      <c r="G71" s="33"/>
+      <c r="A71" s="3">
+        <v>2</v>
+      </c>
+      <c r="B71" s="56"/>
+      <c r="C71" s="7">
+        <v>20230816001</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="G71" s="7">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="H71" s="3">
+        <v>25</v>
+      </c>
+      <c r="I71" s="7">
+        <f>I45+H71-G71</f>
+        <v>27.86</v>
+      </c>
+      <c r="J71" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>3</v>
+      </c>
+      <c r="B72" s="56"/>
+      <c r="C72" s="7">
+        <v>20230816001</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F72" s="8"/>
+      <c r="G72" s="7">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="H72" s="7">
+        <v>25</v>
+      </c>
+      <c r="I72" s="3">
+        <f>I46+H72-G72</f>
+        <v>27.86</v>
+      </c>
+      <c r="J72" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>4</v>
+      </c>
+      <c r="B73" s="56"/>
+      <c r="C73" s="7">
+        <v>20230816002</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F73" s="8"/>
+      <c r="G73" s="7">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="H73" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I73" s="3">
+        <f>I71-G73</f>
+        <v>23.38</v>
+      </c>
+      <c r="J73" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>5</v>
+      </c>
+      <c r="B74" s="56"/>
+      <c r="C74" s="7">
+        <v>20230816002</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F74" s="8"/>
+      <c r="G74" s="7">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="H74" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I74" s="3">
+        <f>I72-G74</f>
+        <v>23.38</v>
+      </c>
+      <c r="J74" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>6</v>
+      </c>
+      <c r="B75" s="56"/>
+      <c r="C75" s="7">
+        <v>20230816003</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F75" s="8"/>
+      <c r="G75" s="7">
+        <v>13.57</v>
+      </c>
+      <c r="H75" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I75" s="37">
+        <f>I73-G75</f>
+        <v>9.8099999999999987</v>
+      </c>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="6">
+        <v>7</v>
+      </c>
+      <c r="B76" s="57"/>
+      <c r="C76" s="9">
+        <v>20230816003</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F76" s="32"/>
+      <c r="G76" s="9">
+        <v>13.57</v>
+      </c>
+      <c r="H76" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="I76" s="44">
+        <f>I74-G76</f>
+        <v>9.8099999999999987</v>
+      </c>
+      <c r="J76" s="6"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="45">
+        <v>1</v>
+      </c>
+      <c r="B77" s="55">
+        <v>45161</v>
+      </c>
+      <c r="C77" s="45">
+        <v>20230816001</v>
+      </c>
+      <c r="D77" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="G77" s="45">
+        <v>30.4</v>
+      </c>
+      <c r="H77" s="45">
+        <v>42.12</v>
+      </c>
+      <c r="I77" s="45">
+        <f>I29+H77-G77</f>
+        <v>14.409999999999997</v>
+      </c>
+      <c r="J77" s="46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>2</v>
+      </c>
+      <c r="B78" s="56"/>
+      <c r="C78" s="3">
+        <v>20230816002</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78" s="3">
+        <v>7.54</v>
+      </c>
+      <c r="H78" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I78" s="3">
+        <f>I77-G78</f>
+        <v>6.8699999999999966</v>
+      </c>
+      <c r="J78" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="6">
+        <v>3</v>
+      </c>
+      <c r="B79" s="57"/>
+      <c r="C79" s="6">
+        <v>20230816003</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G79" s="9">
+        <v>22.78</v>
+      </c>
+      <c r="H79" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="I79" s="44">
+        <f>I78-G79</f>
+        <v>-15.910000000000004</v>
+      </c>
+      <c r="J79" s="6"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="29">
+        <v>1</v>
+      </c>
+      <c r="B80" s="71">
+        <v>45162</v>
+      </c>
+      <c r="C80" s="29">
+        <v>20230816001</v>
+      </c>
+      <c r="D80" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F80" s="72"/>
+      <c r="G80" s="29">
+        <v>321.70999999999998</v>
+      </c>
+      <c r="H80" s="30">
+        <v>250</v>
+      </c>
+      <c r="I80" s="74">
+        <f>H80-G80</f>
+        <v>-71.70999999999998</v>
+      </c>
+      <c r="J80" s="19"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="7">
+        <v>2</v>
+      </c>
+      <c r="B81" s="70"/>
+      <c r="C81" s="7">
+        <v>20230816001</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F81" s="8"/>
+      <c r="G81" s="7">
+        <v>16.37</v>
+      </c>
+      <c r="H81" s="3">
+        <v>25</v>
+      </c>
+      <c r="I81" s="3">
+        <f>I47+H81-G81</f>
+        <v>24.599999999999998</v>
+      </c>
+      <c r="J81" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
+        <v>3</v>
+      </c>
+      <c r="B82" s="70"/>
+      <c r="C82" s="7">
+        <v>20230816002</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F82" s="8"/>
+      <c r="G82" s="7">
+        <v>79.8</v>
+      </c>
+      <c r="H82" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I82" s="36">
+        <f>I80-G82</f>
+        <v>-151.51</v>
+      </c>
+      <c r="J82" s="8"/>
+    </row>
+    <row r="83" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="9">
+        <v>4</v>
+      </c>
+      <c r="B83" s="73"/>
+      <c r="C83" s="9">
+        <v>20230816002</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F83" s="32"/>
+      <c r="G83" s="9">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H83" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="I83" s="44">
+        <f>I81-G83</f>
+        <v>20.54</v>
+      </c>
+      <c r="J83" s="32"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:J68"/>
-  <mergeCells count="30">
-    <mergeCell ref="B51:B69"/>
+  <mergeCells count="33">
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="C39:C44"/>
+    <mergeCell ref="C45:C50"/>
+    <mergeCell ref="B32:B50"/>
+    <mergeCell ref="C29:C30"/>
     <mergeCell ref="C7:C16"/>
     <mergeCell ref="B7:B16"/>
     <mergeCell ref="C27:C28"/>
@@ -2899,11 +3331,6 @@
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="B18:B30"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="C39:C44"/>
-    <mergeCell ref="C45:C50"/>
-    <mergeCell ref="B32:B50"/>
-    <mergeCell ref="C29:C30"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A1:J3"/>
     <mergeCell ref="G4:G5"/>
@@ -2915,12 +3342,15 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="I4:I5"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="B70:B76"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="B51:B69"/>
     <mergeCell ref="C51:C53"/>
     <mergeCell ref="C54:C56"/>
     <mergeCell ref="C57:C59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>